<commit_message>
Final Update Timeplan and apparently dome stuff doku
</commit_message>
<xml_diff>
--- a/Documentation/M223Zeitplan.xlsx
+++ b/Documentation/M223Zeitplan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C30D4CF-9A57-48F0-8AFA-60EFF6761B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C864EBA0-6160-4559-B710-B8690925D6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Arbeit</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Finalisierung und Abgabe</t>
+  </si>
+  <si>
+    <t>NO ZB</t>
   </si>
 </sst>
 </file>
@@ -261,7 +264,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,8 +313,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="70">
+  <borders count="76">
     <border>
       <left/>
       <right/>
@@ -372,19 +381,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -446,17 +442,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -468,10 +453,92 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -487,123 +554,8 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -966,19 +918,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1192,7 +1131,147 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -1208,297 +1287,310 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="59" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="63" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="64" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="66" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="67" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="68" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="69" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="65" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="70" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="64" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1811,10 +1903,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z47"/>
+  <dimension ref="A1:AA47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="Z31" sqref="Z31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,89 +1918,91 @@
     <col min="6" max="10" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.42578125" customWidth="1"/>
     <col min="12" max="18" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="6.5703125" customWidth="1"/>
-    <col min="21" max="21" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="4.42578125" customWidth="1"/>
+    <col min="22" max="22" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="128" t="s">
+      <c r="B1" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="108"/>
-      <c r="D1" s="137" t="s">
+      <c r="C1" s="117"/>
+      <c r="D1" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="137" t="s">
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="137" t="s">
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="137" t="s">
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="138"/>
-      <c r="O1" s="138"/>
-      <c r="P1" s="137" t="s">
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="138"/>
-      <c r="R1" s="138"/>
-      <c r="S1" s="137" t="s">
+      <c r="Q1" s="103"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="138"/>
-      <c r="U1" s="131" t="s">
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="147" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="126"/>
-      <c r="B2" s="129"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="134">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="114"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="100">
         <v>44999</v>
       </c>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="134">
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="100">
         <v>45000</v>
       </c>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="134">
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="100">
         <v>45002</v>
       </c>
-      <c r="K2" s="135"/>
-      <c r="L2" s="135"/>
-      <c r="M2" s="134">
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="100">
         <v>45006</v>
       </c>
-      <c r="N2" s="135"/>
-      <c r="O2" s="135"/>
-      <c r="P2" s="134">
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="100">
         <v>45007</v>
       </c>
-      <c r="Q2" s="135"/>
-      <c r="R2" s="135"/>
-      <c r="S2" s="134">
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101"/>
+      <c r="S2" s="136">
         <v>45009</v>
       </c>
-      <c r="T2" s="136"/>
-      <c r="U2" s="132"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="127"/>
+      <c r="T2" s="137"/>
+      <c r="U2" s="137"/>
+      <c r="V2" s="148"/>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="115"/>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1966,16 +2060,19 @@
       <c r="T3" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="U3" s="133"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="111" t="s">
+      <c r="U3" s="138" t="s">
+        <v>49</v>
+      </c>
+      <c r="V3" s="149"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="113">
+      <c r="B4" s="121">
         <v>1</v>
       </c>
-      <c r="C4" s="115"/>
+      <c r="C4" s="122"/>
       <c r="D4" s="45"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -1993,12 +2090,13 @@
       <c r="R4" s="11"/>
       <c r="S4" s="13"/>
       <c r="T4" s="72"/>
-      <c r="U4" s="109"/>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="103"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="107"/>
+      <c r="U4" s="139"/>
+      <c r="V4" s="150"/>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="110"/>
+      <c r="B5" s="111"/>
+      <c r="C5" s="112"/>
       <c r="D5" s="44"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
@@ -2016,16 +2114,17 @@
       <c r="R5" s="16"/>
       <c r="S5" s="15"/>
       <c r="T5" s="73"/>
-      <c r="U5" s="109"/>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="111" t="s">
+      <c r="U5" s="140"/>
+      <c r="V5" s="150"/>
+    </row>
+    <row r="6" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="113">
+      <c r="B6" s="121">
         <v>1</v>
       </c>
-      <c r="C6" s="115"/>
+      <c r="C6" s="122"/>
       <c r="D6" s="45"/>
       <c r="E6" s="11"/>
       <c r="F6" s="28"/>
@@ -2043,19 +2142,20 @@
       <c r="R6" s="11"/>
       <c r="S6" s="13"/>
       <c r="T6" s="72"/>
-      <c r="U6" s="109"/>
-      <c r="W6" s="58" t="s">
+      <c r="U6" s="139"/>
+      <c r="V6" s="150"/>
+      <c r="X6" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="X6" s="142" t="s">
+      <c r="Y6" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="Y6" s="142"/>
-    </row>
-    <row r="7" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="103"/>
-      <c r="B7" s="105"/>
-      <c r="C7" s="107"/>
+      <c r="Z6" s="99"/>
+    </row>
+    <row r="7" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="110"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="112"/>
       <c r="D7" s="44"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
@@ -2073,23 +2173,24 @@
       <c r="R7" s="16"/>
       <c r="S7" s="15"/>
       <c r="T7" s="73"/>
-      <c r="U7" s="109"/>
-      <c r="W7" s="59" t="s">
+      <c r="U7" s="140"/>
+      <c r="V7" s="150"/>
+      <c r="X7" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="X7" s="142" t="s">
+      <c r="Y7" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="Y7" s="142"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="111" t="s">
+      <c r="Z7" s="99"/>
+    </row>
+    <row r="8" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="113">
+      <c r="B8" s="121">
         <v>1</v>
       </c>
-      <c r="C8" s="115"/>
+      <c r="C8" s="122"/>
       <c r="D8" s="29"/>
       <c r="E8" s="11"/>
       <c r="F8" s="3"/>
@@ -2107,19 +2208,20 @@
       <c r="R8" s="11"/>
       <c r="S8" s="13"/>
       <c r="T8" s="72"/>
-      <c r="U8" s="109"/>
-      <c r="W8" s="60" t="s">
+      <c r="U8" s="139"/>
+      <c r="V8" s="150"/>
+      <c r="X8" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="X8" s="142" t="s">
+      <c r="Y8" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="Y8" s="142"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="112"/>
-      <c r="B9" s="114"/>
-      <c r="C9" s="116"/>
+      <c r="Z8" s="99"/>
+    </row>
+    <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="105"/>
+      <c r="B9" s="107"/>
+      <c r="C9" s="109"/>
       <c r="D9" s="30"/>
       <c r="E9" s="31"/>
       <c r="F9" s="57"/>
@@ -2137,16 +2239,17 @@
       <c r="R9" s="31"/>
       <c r="S9" s="32"/>
       <c r="T9" s="74"/>
-      <c r="U9" s="110"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="102" t="s">
+      <c r="U9" s="141"/>
+      <c r="V9" s="151"/>
+    </row>
+    <row r="10" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="104">
+      <c r="B10" s="106">
         <v>1</v>
       </c>
-      <c r="C10" s="106"/>
+      <c r="C10" s="108"/>
       <c r="D10" s="35"/>
       <c r="E10" s="47"/>
       <c r="F10" s="36"/>
@@ -2164,14 +2267,15 @@
       <c r="R10" s="36"/>
       <c r="S10" s="37"/>
       <c r="T10" s="75"/>
-      <c r="U10" s="108" t="s">
+      <c r="U10" s="142"/>
+      <c r="V10" s="152" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="103"/>
-      <c r="B11" s="105"/>
-      <c r="C11" s="107"/>
+    <row r="11" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="110"/>
+      <c r="B11" s="111"/>
+      <c r="C11" s="112"/>
       <c r="D11" s="52"/>
       <c r="E11" s="64"/>
       <c r="F11" s="19"/>
@@ -2189,20 +2293,21 @@
       <c r="R11" s="19"/>
       <c r="S11" s="18"/>
       <c r="T11" s="76"/>
-      <c r="U11" s="109"/>
-      <c r="W11" s="5" t="s">
+      <c r="U11" s="143"/>
+      <c r="V11" s="150"/>
+      <c r="X11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="X11" s="6"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="111" t="s">
+      <c r="Y11" s="6"/>
+    </row>
+    <row r="12" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="113">
+      <c r="B12" s="121">
         <v>0.5</v>
       </c>
-      <c r="C12" s="115"/>
+      <c r="C12" s="122"/>
       <c r="D12" s="49"/>
       <c r="E12" s="50"/>
       <c r="F12" s="22"/>
@@ -2220,16 +2325,17 @@
       <c r="R12" s="22"/>
       <c r="S12" s="21"/>
       <c r="T12" s="77"/>
-      <c r="U12" s="109"/>
-      <c r="W12" s="5" t="s">
+      <c r="U12" s="144"/>
+      <c r="V12" s="150"/>
+      <c r="X12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="X12" s="7"/>
-    </row>
-    <row r="13" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="112"/>
-      <c r="B13" s="114"/>
-      <c r="C13" s="116"/>
+      <c r="Y12" s="7"/>
+    </row>
+    <row r="13" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="105"/>
+      <c r="B13" s="107"/>
+      <c r="C13" s="109"/>
       <c r="D13" s="30"/>
       <c r="E13" s="57"/>
       <c r="F13" s="31"/>
@@ -2247,20 +2353,21 @@
       <c r="R13" s="31"/>
       <c r="S13" s="32"/>
       <c r="T13" s="74"/>
-      <c r="U13" s="110"/>
-      <c r="W13" s="5" t="s">
+      <c r="U13" s="141"/>
+      <c r="V13" s="151"/>
+      <c r="X13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="X13" s="8"/>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="102" t="s">
+      <c r="Y13" s="8"/>
+    </row>
+    <row r="14" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="104">
+      <c r="B14" s="106">
         <v>2</v>
       </c>
-      <c r="C14" s="106"/>
+      <c r="C14" s="108"/>
       <c r="D14" s="35"/>
       <c r="E14" s="47"/>
       <c r="F14" s="36"/>
@@ -2278,14 +2385,15 @@
       <c r="R14" s="36"/>
       <c r="S14" s="37"/>
       <c r="T14" s="75"/>
-      <c r="U14" s="108" t="s">
+      <c r="U14" s="142"/>
+      <c r="V14" s="152" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="103"/>
-      <c r="B15" s="105"/>
-      <c r="C15" s="107"/>
+    <row r="15" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="110"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="112"/>
       <c r="D15" s="52"/>
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
@@ -2303,22 +2411,23 @@
       <c r="R15" s="19"/>
       <c r="S15" s="18"/>
       <c r="T15" s="76"/>
-      <c r="U15" s="109"/>
-      <c r="W15" s="99" t="s">
+      <c r="U15" s="143"/>
+      <c r="V15" s="150"/>
+      <c r="X15" s="125" t="s">
         <v>43</v>
       </c>
-      <c r="X15" s="100"/>
-      <c r="Y15" s="100"/>
-      <c r="Z15" s="101"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="111" t="s">
+      <c r="Y15" s="126"/>
+      <c r="Z15" s="126"/>
+      <c r="AA15" s="127"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="120" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="113">
+      <c r="B16" s="121">
         <v>1</v>
       </c>
-      <c r="C16" s="115"/>
+      <c r="C16" s="122"/>
       <c r="D16" s="29"/>
       <c r="E16" s="11"/>
       <c r="F16" s="3"/>
@@ -2336,18 +2445,19 @@
       <c r="R16" s="11"/>
       <c r="S16" s="13"/>
       <c r="T16" s="72"/>
-      <c r="U16" s="109"/>
-      <c r="W16" s="139" t="s">
+      <c r="U16" s="139"/>
+      <c r="V16" s="150"/>
+      <c r="X16" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="X16" s="140"/>
-      <c r="Y16" s="140"/>
-      <c r="Z16" s="141"/>
-    </row>
-    <row r="17" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="103"/>
-      <c r="B17" s="105"/>
-      <c r="C17" s="107"/>
+      <c r="Y16" s="97"/>
+      <c r="Z16" s="97"/>
+      <c r="AA16" s="98"/>
+    </row>
+    <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="110"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="112"/>
       <c r="D17" s="52"/>
       <c r="E17" s="19"/>
       <c r="F17" s="65"/>
@@ -2365,22 +2475,23 @@
       <c r="R17" s="19"/>
       <c r="S17" s="18"/>
       <c r="T17" s="76"/>
-      <c r="U17" s="109"/>
-      <c r="W17" s="139" t="s">
+      <c r="U17" s="143"/>
+      <c r="V17" s="150"/>
+      <c r="X17" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="X17" s="140"/>
-      <c r="Y17" s="140"/>
-      <c r="Z17" s="141"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" s="111" t="s">
+      <c r="Y17" s="97"/>
+      <c r="Z17" s="97"/>
+      <c r="AA17" s="98"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="113">
+      <c r="B18" s="121">
         <v>1</v>
       </c>
-      <c r="C18" s="115"/>
+      <c r="C18" s="122"/>
       <c r="D18" s="29"/>
       <c r="E18" s="11"/>
       <c r="F18" s="3"/>
@@ -2398,12 +2509,13 @@
       <c r="R18" s="11"/>
       <c r="S18" s="13"/>
       <c r="T18" s="72"/>
-      <c r="U18" s="109"/>
-    </row>
-    <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="103"/>
-      <c r="B19" s="105"/>
-      <c r="C19" s="107"/>
+      <c r="U18" s="139"/>
+      <c r="V18" s="150"/>
+    </row>
+    <row r="19" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="110"/>
+      <c r="B19" s="111"/>
+      <c r="C19" s="112"/>
       <c r="D19" s="52"/>
       <c r="E19" s="19"/>
       <c r="F19" s="64"/>
@@ -2421,16 +2533,17 @@
       <c r="R19" s="19"/>
       <c r="S19" s="18"/>
       <c r="T19" s="76"/>
-      <c r="U19" s="109"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="111" t="s">
+      <c r="U19" s="143"/>
+      <c r="V19" s="150"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="113">
+      <c r="B20" s="121">
         <v>1</v>
       </c>
-      <c r="C20" s="115"/>
+      <c r="C20" s="122"/>
       <c r="D20" s="49"/>
       <c r="E20" s="50"/>
       <c r="G20" s="21"/>
@@ -2447,12 +2560,13 @@
       <c r="R20" s="22"/>
       <c r="S20" s="21"/>
       <c r="T20" s="77"/>
-      <c r="U20" s="109"/>
-    </row>
-    <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="112"/>
-      <c r="B21" s="114"/>
-      <c r="C21" s="116"/>
+      <c r="U20" s="144"/>
+      <c r="V20" s="150"/>
+    </row>
+    <row r="21" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="105"/>
+      <c r="B21" s="107"/>
+      <c r="C21" s="109"/>
       <c r="D21" s="30"/>
       <c r="E21" s="31"/>
       <c r="F21" s="31"/>
@@ -2470,16 +2584,17 @@
       <c r="R21" s="31"/>
       <c r="S21" s="32"/>
       <c r="T21" s="74"/>
-      <c r="U21" s="110"/>
-    </row>
-    <row r="22" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="102" t="s">
+      <c r="U21" s="141"/>
+      <c r="V21" s="151"/>
+    </row>
+    <row r="22" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="104">
+      <c r="B22" s="106">
         <v>0.5</v>
       </c>
-      <c r="C22" s="106"/>
+      <c r="C22" s="108"/>
       <c r="D22" s="35"/>
       <c r="E22" s="36"/>
       <c r="F22" s="47"/>
@@ -2497,14 +2612,15 @@
       <c r="R22" s="36"/>
       <c r="S22" s="37"/>
       <c r="T22" s="75"/>
-      <c r="U22" s="108" t="s">
+      <c r="U22" s="142"/>
+      <c r="V22" s="152" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="112"/>
-      <c r="B23" s="114"/>
-      <c r="C23" s="116"/>
+    <row r="23" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="105"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="109"/>
       <c r="D23" s="30"/>
       <c r="E23" s="31"/>
       <c r="F23" s="57"/>
@@ -2522,16 +2638,17 @@
       <c r="R23" s="31"/>
       <c r="S23" s="32"/>
       <c r="T23" s="74"/>
-      <c r="U23" s="110"/>
-    </row>
-    <row r="24" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="102" t="s">
+      <c r="U23" s="141"/>
+      <c r="V23" s="151"/>
+    </row>
+    <row r="24" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="104">
+      <c r="B24" s="106">
         <v>1</v>
       </c>
-      <c r="C24" s="106"/>
+      <c r="C24" s="108"/>
       <c r="D24" s="46"/>
       <c r="E24" s="36"/>
       <c r="F24" s="36"/>
@@ -2549,14 +2666,15 @@
       <c r="R24" s="36"/>
       <c r="S24" s="37"/>
       <c r="T24" s="75"/>
-      <c r="U24" s="108" t="s">
+      <c r="U24" s="142"/>
+      <c r="V24" s="152" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="103"/>
-      <c r="B25" s="105"/>
-      <c r="C25" s="107"/>
+    <row r="25" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="110"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="112"/>
       <c r="D25" s="54"/>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
@@ -2574,16 +2692,17 @@
       <c r="R25" s="19"/>
       <c r="S25" s="18"/>
       <c r="T25" s="76"/>
-      <c r="U25" s="109"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="111" t="s">
+      <c r="U25" s="143"/>
+      <c r="V25" s="150"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="113">
+      <c r="B26" s="121">
         <v>1</v>
       </c>
-      <c r="C26" s="115"/>
+      <c r="C26" s="122"/>
       <c r="D26" s="29"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
@@ -2601,12 +2720,13 @@
       <c r="R26" s="11"/>
       <c r="S26" s="13"/>
       <c r="T26" s="72"/>
-      <c r="U26" s="109"/>
-    </row>
-    <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="103"/>
-      <c r="B27" s="105"/>
-      <c r="C27" s="107"/>
+      <c r="U26" s="139"/>
+      <c r="V26" s="150"/>
+    </row>
+    <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="110"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="112"/>
       <c r="D27" s="52"/>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
@@ -2624,16 +2744,17 @@
       <c r="R27" s="19"/>
       <c r="S27" s="18"/>
       <c r="T27" s="76"/>
-      <c r="U27" s="109"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="111" t="s">
+      <c r="U27" s="143"/>
+      <c r="V27" s="150"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28" s="120" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="113">
+      <c r="B28" s="121">
         <v>2</v>
       </c>
-      <c r="C28" s="115"/>
+      <c r="C28" s="122"/>
       <c r="D28" s="29"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
@@ -2651,12 +2772,13 @@
       <c r="R28" s="11"/>
       <c r="S28" s="13"/>
       <c r="T28" s="72"/>
-      <c r="U28" s="109"/>
-    </row>
-    <row r="29" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="103"/>
-      <c r="B29" s="105"/>
-      <c r="C29" s="107"/>
+      <c r="U28" s="139"/>
+      <c r="V28" s="150"/>
+    </row>
+    <row r="29" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="110"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="112"/>
       <c r="D29" s="52"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
@@ -2672,18 +2794,19 @@
       <c r="P29" s="18"/>
       <c r="Q29" s="19"/>
       <c r="R29" s="19"/>
-      <c r="S29" s="18"/>
+      <c r="S29" s="66"/>
       <c r="T29" s="76"/>
-      <c r="U29" s="109"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="111" t="s">
+      <c r="U29" s="143"/>
+      <c r="V29" s="150"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="113">
+      <c r="B30" s="121">
         <v>3</v>
       </c>
-      <c r="C30" s="115"/>
+      <c r="C30" s="122"/>
       <c r="D30" s="29"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
@@ -2701,12 +2824,13 @@
       <c r="R30" s="11"/>
       <c r="S30" s="13"/>
       <c r="T30" s="72"/>
-      <c r="U30" s="109"/>
-    </row>
-    <row r="31" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="103"/>
-      <c r="B31" s="105"/>
-      <c r="C31" s="107"/>
+      <c r="U30" s="139"/>
+      <c r="V30" s="150"/>
+    </row>
+    <row r="31" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="110"/>
+      <c r="B31" s="111"/>
+      <c r="C31" s="112"/>
       <c r="D31" s="52"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
@@ -2722,18 +2846,19 @@
       <c r="P31" s="18"/>
       <c r="Q31" s="19"/>
       <c r="R31" s="19"/>
-      <c r="S31" s="18"/>
+      <c r="S31" s="66"/>
       <c r="T31" s="76"/>
-      <c r="U31" s="109"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" s="111" t="s">
+      <c r="U31" s="143"/>
+      <c r="V31" s="150"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="113">
+      <c r="B32" s="121">
         <v>2</v>
       </c>
-      <c r="C32" s="115"/>
+      <c r="C32" s="122"/>
       <c r="D32" s="29"/>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
@@ -2751,12 +2876,13 @@
       <c r="R32" s="11"/>
       <c r="S32" s="13"/>
       <c r="T32" s="72"/>
-      <c r="U32" s="109"/>
-    </row>
-    <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="103"/>
-      <c r="B33" s="105"/>
-      <c r="C33" s="107"/>
+      <c r="U32" s="139"/>
+      <c r="V32" s="150"/>
+    </row>
+    <row r="33" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="110"/>
+      <c r="B33" s="111"/>
+      <c r="C33" s="112"/>
       <c r="D33" s="52"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
@@ -2773,17 +2899,18 @@
       <c r="Q33" s="19"/>
       <c r="R33" s="19"/>
       <c r="S33" s="18"/>
-      <c r="T33" s="76"/>
-      <c r="U33" s="109"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T33" s="135"/>
+      <c r="U33" s="143"/>
+      <c r="V33" s="150"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="113">
+      <c r="B34" s="121">
         <v>2</v>
       </c>
-      <c r="C34" s="115"/>
+      <c r="C34" s="122"/>
       <c r="D34" s="29"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
@@ -2801,12 +2928,13 @@
       <c r="R34" s="11"/>
       <c r="S34" s="13"/>
       <c r="T34" s="72"/>
-      <c r="U34" s="109"/>
-    </row>
-    <row r="35" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U34" s="139"/>
+      <c r="V34" s="150"/>
+    </row>
+    <row r="35" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="124"/>
-      <c r="B35" s="105"/>
-      <c r="C35" s="107"/>
+      <c r="B35" s="111"/>
+      <c r="C35" s="112"/>
       <c r="D35" s="52"/>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
@@ -2823,17 +2951,18 @@
       <c r="Q35" s="19"/>
       <c r="R35" s="19"/>
       <c r="S35" s="18"/>
-      <c r="T35" s="76"/>
-      <c r="U35" s="109"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="111" t="s">
+      <c r="T35" s="135"/>
+      <c r="U35" s="143"/>
+      <c r="V35" s="150"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="120" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="113">
+      <c r="B36" s="121">
         <v>4</v>
       </c>
-      <c r="C36" s="115"/>
+      <c r="C36" s="122"/>
       <c r="D36" s="49"/>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
@@ -2851,12 +2980,13 @@
       <c r="R36" s="22"/>
       <c r="S36" s="21"/>
       <c r="T36" s="77"/>
-      <c r="U36" s="109"/>
-    </row>
-    <row r="37" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="112"/>
-      <c r="B37" s="114"/>
-      <c r="C37" s="116"/>
+      <c r="U36" s="144"/>
+      <c r="V36" s="150"/>
+    </row>
+    <row r="37" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="105"/>
+      <c r="B37" s="107"/>
+      <c r="C37" s="109"/>
       <c r="D37" s="30"/>
       <c r="E37" s="31"/>
       <c r="F37" s="31"/>
@@ -2874,16 +3004,17 @@
       <c r="R37" s="31"/>
       <c r="S37" s="32"/>
       <c r="T37" s="74"/>
-      <c r="U37" s="110"/>
-    </row>
-    <row r="38" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="102" t="s">
+      <c r="U37" s="141"/>
+      <c r="V37" s="151"/>
+    </row>
+    <row r="38" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="104">
+      <c r="B38" s="106">
         <v>0.5</v>
       </c>
-      <c r="C38" s="106"/>
+      <c r="C38" s="108"/>
       <c r="D38" s="35"/>
       <c r="E38" s="36"/>
       <c r="F38" s="36"/>
@@ -2901,14 +3032,15 @@
       <c r="R38" s="36"/>
       <c r="S38" s="37"/>
       <c r="T38" s="75"/>
-      <c r="U38" s="108" t="s">
+      <c r="U38" s="142"/>
+      <c r="V38" s="152" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="103"/>
-      <c r="B39" s="105"/>
-      <c r="C39" s="107"/>
+    <row r="39" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="110"/>
+      <c r="B39" s="111"/>
+      <c r="C39" s="112"/>
       <c r="D39" s="52"/>
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
@@ -2926,16 +3058,17 @@
       <c r="R39" s="19"/>
       <c r="S39" s="18"/>
       <c r="T39" s="76"/>
-      <c r="U39" s="109"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="111" t="s">
+      <c r="U39" s="143"/>
+      <c r="V39" s="150"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="113">
+      <c r="B40" s="121">
         <v>2</v>
       </c>
-      <c r="C40" s="115"/>
+      <c r="C40" s="122"/>
       <c r="D40" s="49"/>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
@@ -2953,12 +3086,13 @@
       <c r="R40" s="22"/>
       <c r="S40" s="21"/>
       <c r="T40" s="77"/>
-      <c r="U40" s="109"/>
-    </row>
-    <row r="41" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="112"/>
-      <c r="B41" s="114"/>
-      <c r="C41" s="116"/>
+      <c r="U40" s="144"/>
+      <c r="V40" s="150"/>
+    </row>
+    <row r="41" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="105"/>
+      <c r="B41" s="107"/>
+      <c r="C41" s="109"/>
       <c r="D41" s="30"/>
       <c r="E41" s="31"/>
       <c r="F41" s="31"/>
@@ -2976,16 +3110,17 @@
       <c r="R41" s="57"/>
       <c r="S41" s="32"/>
       <c r="T41" s="74"/>
-      <c r="U41" s="110"/>
-    </row>
-    <row r="42" spans="1:21" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="102" t="s">
+      <c r="U41" s="141"/>
+      <c r="V41" s="151"/>
+    </row>
+    <row r="42" spans="1:22" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="B42" s="104">
+      <c r="B42" s="106">
         <v>1</v>
       </c>
-      <c r="C42" s="119"/>
+      <c r="C42" s="130"/>
       <c r="D42" s="35"/>
       <c r="E42" s="36"/>
       <c r="F42" s="36"/>
@@ -3003,14 +3138,15 @@
       <c r="R42" s="36"/>
       <c r="S42" s="48"/>
       <c r="T42" s="78"/>
-      <c r="U42" s="96" t="s">
+      <c r="U42" s="142"/>
+      <c r="V42" s="152" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="117"/>
-      <c r="B43" s="118"/>
-      <c r="C43" s="120"/>
+    <row r="43" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="128"/>
+      <c r="B43" s="129"/>
+      <c r="C43" s="131"/>
       <c r="D43" s="80"/>
       <c r="E43" s="81"/>
       <c r="F43" s="81"/>
@@ -3028,13 +3164,14 @@
       <c r="R43" s="81"/>
       <c r="S43" s="82"/>
       <c r="T43" s="86"/>
-      <c r="U43" s="97"/>
-    </row>
-    <row r="44" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="102" t="s">
+      <c r="U43" s="145"/>
+      <c r="V43" s="150"/>
+    </row>
+    <row r="44" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="104" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="104">
+      <c r="B44" s="106">
         <v>2</v>
       </c>
       <c r="C44" s="87"/>
@@ -3055,11 +3192,12 @@
       <c r="R44" s="89"/>
       <c r="S44" s="90"/>
       <c r="T44" s="95"/>
-      <c r="U44" s="97"/>
-    </row>
-    <row r="45" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="121"/>
-      <c r="B45" s="122"/>
+      <c r="U44" s="146"/>
+      <c r="V44" s="150"/>
+    </row>
+    <row r="45" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="132"/>
+      <c r="B45" s="133"/>
       <c r="C45" s="94"/>
       <c r="D45" s="30"/>
       <c r="E45" s="31"/>
@@ -3077,10 +3215,11 @@
       <c r="Q45" s="31"/>
       <c r="R45" s="31"/>
       <c r="S45" s="32"/>
-      <c r="T45" s="74"/>
-      <c r="U45" s="98"/>
-    </row>
-    <row r="46" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T45" s="134"/>
+      <c r="U45" s="141"/>
+      <c r="V45" s="153"/>
+    </row>
+    <row r="46" spans="1:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>28</v>
       </c>
@@ -3093,44 +3232,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="W17:Z17"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="W16:Z16"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="U10:U13"/>
+    <mergeCell ref="V42:V45"/>
+    <mergeCell ref="X15:AA15"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="V38:V41"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="V22:V23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="V24:V37"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="V14:V21"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="V10:V13"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
-    <mergeCell ref="U4:U9"/>
+    <mergeCell ref="V4:V9"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
@@ -3142,50 +3295,36 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="U14:U21"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="U22:U23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="U24:U37"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="U42:U45"/>
-    <mergeCell ref="W15:Z15"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="U38:U41"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="X17:AA17"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="X16:AA16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="59" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>